<commit_message>
REPORTGEN-1021: update report template
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Sizing reports/AEP-sample-Template.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Sizing reports/AEP-sample-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Sizing reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924D785F-C113-4EF1-8DC2-710674A51A1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D648C7-88B0-4D34-891F-4A6B479EE060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2505" windowWidth="21075" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2505" windowWidth="21075" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E5470F-AD14-42F3-8810-0BAE0FBFD299}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REPORTGEN-967: limit number of rows in aep_sample template
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Sizing reports/AEP-sample-Template.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Sizing reports/AEP-sample-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Sizing reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Sizing reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F79EFD-4F7A-45A4-885A-6E03AEF86F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE656D-B5B6-41BD-A8BF-21D5729EEAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -117,13 +117,13 @@
     <t>RepGen:TEXT;LAST_SNAPSHOT_VERSION</t>
   </si>
   <si>
-    <t>RepGen:TABLE;AETP_LIST;COUNT=-1,FORMAT=N5</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;AEFP_LIST;TYPE=TF,COUNT=-1,ZERO=NO</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;AEFP_LIST;TYPE=DF,COUNT=-1,ZERO=NO</t>
+    <t>RepGen:TABLE;AEFP_LIST;TYPE=TF,COUNT=5000,ZERO=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;AEFP_LIST;TYPE=DF,COUNT=5000,ZERO=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;AETP_LIST;COUNT=5000,FORMAT=N5</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1264,7 @@
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1380,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1453,7 @@
     <row r="7" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1468,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1540,7 @@
     <row r="7" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +1626,7 @@
     <row r="7" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>